<commit_message>
corrected typo in taxonomy tags.
replace "Interpretating ..." with "Interpreting ...".
</commit_message>
<xml_diff>
--- a/source/Taxonomie ShareStats versie 17 maart 2021.xlsx
+++ b/source/Taxonomie ShareStats versie 17 maart 2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbookprosharon/GitHub/Statistics_Taxonomy/source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shklinkenberg/GitHub/Statistics_Taxonomy/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB724685-C2B3-514F-A4EA-23774131E892}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4606C1-0861-7B48-8442-1141AC81B90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-920" windowWidth="38400" windowHeight="21140" xr2:uid="{02F0BE0C-4641-44B2-84E7-71A771F2B1F3}"/>
+    <workbookView xWindow="1940" yWindow="-20260" windowWidth="30240" windowHeight="18880" activeTab="1" xr2:uid="{02F0BE0C-4641-44B2-84E7-71A771F2B1F3}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistical Topic" sheetId="1" r:id="rId1"/>
@@ -979,13 +979,7 @@
     <t xml:space="preserve">The student is asked to combine data, screen data, create new variables in a dataset, or calculate descriptive statistics using the data supplied with the question. </t>
   </si>
   <si>
-    <t>Interpretating graph</t>
-  </si>
-  <si>
     <t xml:space="preserve">The graph is supplied with the question. The student is asked to look at the graph and describe what is going on, draw conclusions based on the graph, etc. </t>
-  </si>
-  <si>
-    <t>Interpretating output</t>
   </si>
   <si>
     <t xml:space="preserve">The output is either supplied with the question or the student has run an analysis to create the output (combine with "Performing analysis"). The student is asked to look at the output and report results/draw conclusions based on it. </t>
@@ -1097,6 +1091,12 @@
   </si>
   <si>
     <t>NL vertaling</t>
+  </si>
+  <si>
+    <t>Interpreting graph</t>
+  </si>
+  <si>
+    <t>Interpreting output</t>
   </si>
 </sst>
 </file>
@@ -1824,7 +1824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8698F61-1708-4E3E-B3B0-071E2B6F89C4}">
   <dimension ref="A1:G316"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="133" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="133" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
@@ -1861,7 +1861,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -4562,8 +4562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25850259-8A21-42D8-B210-7F91CBE4A0DC}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4648,21 +4648,21 @@
     </row>
     <row r="7" spans="1:13" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="64" t="s">
-        <v>312</v>
+        <v>345</v>
       </c>
       <c r="B7" s="64"/>
       <c r="C7" s="65" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D7" s="65"/>
     </row>
     <row r="8" spans="1:13" ht="80" x14ac:dyDescent="0.2">
       <c r="A8" s="64" t="s">
-        <v>314</v>
+        <v>346</v>
       </c>
       <c r="B8" s="64"/>
       <c r="C8" s="65" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D8" s="65"/>
       <c r="H8" s="50"/>
@@ -4674,11 +4674,11 @@
     </row>
     <row r="9" spans="1:13" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="64" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B9" s="64"/>
       <c r="C9" s="65" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D9" s="65"/>
       <c r="H9" s="50"/>
@@ -4690,20 +4690,20 @@
     </row>
     <row r="10" spans="1:13" ht="160" x14ac:dyDescent="0.2">
       <c r="A10" s="64" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B10" s="64"/>
       <c r="C10" s="65" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D10" s="65" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="M10" s="50"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="64" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B11" s="64"/>
       <c r="C11" s="65"/>
@@ -4713,7 +4713,7 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="64"/>
       <c r="B12" s="64" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C12" s="65"/>
       <c r="D12" s="65"/>
@@ -4722,7 +4722,7 @@
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="64"/>
       <c r="B13" s="64" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C13" s="65"/>
       <c r="D13" s="65"/>
@@ -4730,7 +4730,7 @@
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="64"/>
       <c r="B14" s="64" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C14" s="65"/>
       <c r="D14" s="65"/>
@@ -4738,7 +4738,7 @@
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="64"/>
       <c r="B15" s="64" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C15" s="65"/>
       <c r="D15" s="65"/>
@@ -4746,7 +4746,7 @@
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="64"/>
       <c r="B16" s="63" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C16" s="65"/>
       <c r="D16" s="65"/>
@@ -4754,7 +4754,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="64"/>
       <c r="B17" s="64" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C17" s="65"/>
       <c r="D17" s="65"/>
@@ -4762,14 +4762,14 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="64"/>
       <c r="B18" s="64" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C18" s="65"/>
       <c r="D18" s="65"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="64" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B19" s="64"/>
       <c r="C19" s="65"/>
@@ -4778,7 +4778,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="64"/>
       <c r="B20" s="64" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C20" s="65"/>
       <c r="D20" s="65"/>
@@ -4786,7 +4786,7 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="64"/>
       <c r="B21" s="64" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C21" s="65"/>
       <c r="D21" s="65"/>
@@ -4827,7 +4827,7 @@
   </sheetPr>
   <dimension ref="A1:D993"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -4842,13 +4842,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="60" customFormat="1" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B1" s="59" t="s">
         <v>298</v>
       </c>
       <c r="C1" s="59" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D1" s="59" t="s">
         <v>299</v>
@@ -4856,44 +4856,44 @@
     </row>
     <row r="2" spans="1:4" ht="119" x14ac:dyDescent="0.2">
       <c r="A2" s="56" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>333</v>
+      </c>
+      <c r="C2" s="57" t="s">
         <v>334</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="D2" s="58" t="s">
         <v>335</v>
-      </c>
-      <c r="C2" s="57" t="s">
-        <v>336</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" s="56" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3" s="57" t="s">
+        <v>337</v>
+      </c>
+      <c r="C3" s="57" t="s">
         <v>338</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="D3" s="58" t="s">
         <v>339</v>
-      </c>
-      <c r="C3" s="57" t="s">
-        <v>340</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="256.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="56" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" s="57" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" s="57" t="s">
         <v>342</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="D4" s="58" t="s">
         <v>343</v>
-      </c>
-      <c r="C4" s="57" t="s">
-        <v>344</v>
-      </c>
-      <c r="D4" s="58" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -10037,21 +10037,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B24D943BF42BB54E8E28D33AC457B357" ma:contentTypeVersion="7" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="fac10887ae73272f9b379da038210499">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d061366e-998c-445a-b60d-7475d805239e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a305e04f14c381a389c3eb6e0cbc1f4d" ns2:_="">
     <xsd:import namespace="d061366e-998c-445a-b60d-7475d805239e"/>
@@ -10215,15 +10206,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5080ED9-77C9-414F-BE11-6B10B32C1309}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{191A8A60-E979-4294-8A87-1F84B5009400}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -10239,7 +10231,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56D0AAE0-E0EE-47A2-BD1A-D346AB677788}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10255,4 +10247,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5080ED9-77C9-414F-BE11-6B10B32C1309}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>